<commit_message>
Implemented Avg. line coverage for all the systems and detector, updated paper
</commit_message>
<xml_diff>
--- a/data_files/final_dataset/demo.xlsx
+++ b/data_files/final_dataset/demo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MD NADIM\Documents\NetBeansProjects\FindCochangeByClone\data_files\final_dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdn769\FindCochangeByClone\data_files\final_dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EA8D65-7E31-4395-A200-02776569E088}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDD11B2C-8780-420C-B635-BD410DD62F2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1EAD1D40-6DDA-4BB0-8532-1C1B516C7D8D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1EAD1D40-6DDA-4BB0-8532-1C1B516C7D8D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,24 +469,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A4AFBA-55C8-4828-869F-E35478EED2B4}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="325" zoomScaleNormal="325" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" style="1"/>
+    <col min="6" max="6" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.109375" style="1"/>
+    <col min="9" max="9" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>9</v>
       </c>
@@ -500,7 +500,7 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -526,7 +526,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -554,7 +554,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -582,7 +582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -610,7 +610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -638,7 +638,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -649,7 +649,7 @@
         <v>212</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" ref="D7:D12" si="2">C7-B7+1</f>
+        <f t="shared" ref="D7" si="2">C7-B7+1</f>
         <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -666,7 +666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F8" s="1" t="s">
         <v>17</v>
       </c>
@@ -681,7 +681,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F9" s="1" t="s">
         <v>18</v>
       </c>
@@ -696,7 +696,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F10" s="1" t="s">
         <v>19</v>
       </c>

</xml_diff>